<commit_message>
Esqueleto guión Grado 06 Guión 03
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/esqueletoGuion_CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/esqueletoGuion_CN_06_03_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="88">
   <si>
     <t>FICHA</t>
   </si>
@@ -1525,7 +1525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1535,7 +1535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1778,7 +1778,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1802,7 +1802,9 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -1811,7 +1813,9 @@
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
       <c r="C3">
         <v>2</v>
       </c>
@@ -1820,7 +1824,9 @@
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
       <c r="C4">
         <v>3</v>
       </c>
@@ -1829,7 +1835,9 @@
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
       <c r="C5">
         <v>4</v>
       </c>
@@ -1838,6 +1846,9 @@
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
       <c r="C6">
         <v>5</v>
       </c>
@@ -1846,6 +1857,9 @@
       <c r="A7" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
       <c r="C7">
         <v>6</v>
       </c>
@@ -1854,6 +1868,9 @@
       <c r="A8" t="s">
         <v>38</v>
       </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
       <c r="C8">
         <v>7</v>
       </c>
@@ -1862,6 +1879,9 @@
       <c r="A9" t="s">
         <v>48</v>
       </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
       <c r="C9">
         <v>9</v>
       </c>
@@ -1870,6 +1890,9 @@
       <c r="A10" t="s">
         <v>58</v>
       </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
       <c r="C10">
         <v>11</v>
       </c>
@@ -1878,6 +1901,9 @@
       <c r="A11" t="s">
         <v>59</v>
       </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
       <c r="C11">
         <v>12</v>
       </c>
@@ -1886,6 +1912,9 @@
       <c r="A12" t="s">
         <v>61</v>
       </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
       <c r="C12">
         <v>13</v>
       </c>
@@ -1894,6 +1923,9 @@
       <c r="A13" t="s">
         <v>64</v>
       </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
       <c r="C13">
         <v>14</v>
       </c>
@@ -1902,6 +1934,9 @@
       <c r="A14" t="s">
         <v>69</v>
       </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
       <c r="C14">
         <v>15</v>
       </c>
@@ -1910,6 +1945,9 @@
       <c r="A15" t="s">
         <v>70</v>
       </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
       <c r="C15">
         <v>16</v>
       </c>
@@ -1918,6 +1956,9 @@
       <c r="A16" t="s">
         <v>79</v>
       </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
       <c r="C16">
         <v>19</v>
       </c>
@@ -1926,7 +1967,9 @@
       <c r="A17" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
       <c r="C17" s="18">
         <v>21</v>
       </c>
@@ -1935,7 +1978,9 @@
       <c r="A18" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="18"/>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
       <c r="C18" s="18">
         <v>22</v>
       </c>
@@ -2247,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
     </sheetView>

</xml_diff>